<commit_message>
Update pricing model to include datamart
Do this because they purchased it.
</commit_message>
<xml_diff>
--- a/0273NYP - New York Premier/0273UAB - University of Alabama Birmingham/Pricing_Model_0273UAB_2018-02-21.xlsx
+++ b/0273NYP - New York Premier/0273UAB - University of Alabama Birmingham/Pricing_Model_0273UAB_2018-02-21.xlsx
@@ -1029,7 +1029,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,7 +1136,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="56" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E8" s="56"/>
       <c r="F8" s="56"/>
@@ -1453,7 +1453,7 @@
       </c>
       <c r="D8" s="16">
         <f>SUM(Calcs!D36, Calcs!D49)</f>
-        <v>0</v>
+        <v>6750</v>
       </c>
       <c r="E8" s="16">
         <f>SUM(Calcs!E36, Calcs!E49)</f>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="D30" s="7">
         <f>SUM(D7:D17, D20:D23, D26:D28)</f>
-        <v>92700</v>
+        <v>99450</v>
       </c>
       <c r="E30" s="7">
         <f t="shared" ref="E30:H30" si="0">SUM(E7:E17, E20:E23, E26:E28)</f>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="D35" s="7">
         <f>(D30/12*Inputs!$C$2+D4)*$C$33</f>
-        <v>283100</v>
+        <v>303350</v>
       </c>
       <c r="E35" s="7">
         <f>(E30/12*Inputs!$C$2+E4)*$C$33</f>
@@ -2182,13 +2182,13 @@
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C39" s="7">
         <f>SUM(Outputs_Timeline!S:S)</f>
-        <v>283100</v>
+        <v>303350</v>
       </c>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C40" s="53">
         <f>SUM(D35:H35)</f>
-        <v>283100</v>
+        <v>303350</v>
       </c>
       <c r="D40" s="1"/>
       <c r="G40" s="1"/>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="D9" s="16">
         <f>SUM(Calcs!D10:H10)</f>
-        <v>0</v>
+        <v>6750</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="32">
@@ -2444,11 +2444,11 @@
       </c>
       <c r="K9" s="16">
         <f t="shared" ref="K9:K18" si="3">F9*$D9</f>
-        <v>0</v>
+        <v>1350</v>
       </c>
       <c r="L9" s="16">
         <f t="shared" ref="L9:L17" si="4">G9*$D9</f>
-        <v>0</v>
+        <v>5400</v>
       </c>
       <c r="M9" s="16">
         <f t="shared" si="2"/>
@@ -3720,19 +3720,19 @@
       </c>
       <c r="F49" s="3">
         <f>IFERROR(SUM(K8:K48)/SUM($K8:$N48), 0)</f>
-        <v>0.27784757413423744</v>
+        <v>0.27255831427127009</v>
       </c>
       <c r="G49" s="3">
         <f>IFERROR(SUM(L8:L48)/SUM($K8:$N48), 0)</f>
-        <v>0.68048138603086517</v>
+        <v>0.68860193461282049</v>
       </c>
       <c r="H49" s="3">
         <f>IFERROR(SUM(M8:M48)/SUM($K8:$N48), 0)</f>
-        <v>3.8465575232213139E-2</v>
+        <v>3.5852077953147404E-2</v>
       </c>
       <c r="I49" s="3">
         <f>1-F49-G49-H49</f>
-        <v>3.2054646026842548E-3</v>
+        <v>2.9876731627620223E-3</v>
       </c>
       <c r="K49" s="12">
         <f>F49*$D$49</f>
@@ -3761,19 +3761,19 @@
       </c>
       <c r="F50" s="3">
         <f>IFERROR(SUM(K8:K48)/SUM($K$8:$N48), 0)</f>
-        <v>0.27784757413423744</v>
+        <v>0.27255831427127009</v>
       </c>
       <c r="G50" s="3">
         <f>IFERROR(SUM(L8:L48)/SUM($K$8:$N48), 0)</f>
-        <v>0.68048138603086517</v>
+        <v>0.68860193461282049</v>
       </c>
       <c r="H50" s="3">
         <f>IFERROR(SUM(M8:M48)/SUM($K$8:$N48), 0)</f>
-        <v>3.8465575232213139E-2</v>
+        <v>3.5852077953147404E-2</v>
       </c>
       <c r="I50" s="3">
         <f>1-F50-G50-H50</f>
-        <v>3.2054646026842548E-3</v>
+        <v>2.9876731627620223E-3</v>
       </c>
       <c r="K50" s="80">
         <f>F50*$D$50</f>
@@ -3803,15 +3803,15 @@
       </c>
       <c r="D52" s="1">
         <f>SUM(Outputs_External!D30:'Outputs_External'!H30)</f>
-        <v>92700</v>
+        <v>99450</v>
       </c>
       <c r="K52" s="12">
         <f>SUM(K48:K50, K36:K39, K8:K18,K23:K33,K42:K45)</f>
-        <v>25727.800646868571</v>
+        <v>27077.800646868571</v>
       </c>
       <c r="L52" s="12">
         <f>SUM(L48:L50, L36:L39, L8:L18,L23:L33,L42:L45)</f>
-        <v>63010.4095681201</v>
+        <v>68410.4095681201</v>
       </c>
       <c r="M52" s="12">
         <f>SUM(M48:M50, M36:M39, M8:M18,M23:M33,M42:M45)</f>
@@ -3828,7 +3828,7 @@
       </c>
       <c r="D53" s="23">
         <f>SUM(K52:N52)</f>
-        <v>92596.815815417605</v>
+        <v>99346.815815417605</v>
       </c>
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
@@ -3845,15 +3845,15 @@
       </c>
       <c r="D55" s="1">
         <f>SUM(Outputs_Timeline!S:S)</f>
-        <v>283100</v>
+        <v>303350</v>
       </c>
       <c r="K55" s="12">
         <f>SUM(Outputs_Timeline!T:T)</f>
-        <v>79683.40194060572</v>
+        <v>83733.40194060572</v>
       </c>
       <c r="L55" s="12">
         <f>SUM(Outputs_Timeline!U:U)</f>
-        <v>191531.22870436031</v>
+        <v>207731.22870436031</v>
       </c>
       <c r="M55" s="12">
         <f>SUM(Outputs_Timeline!V:V)</f>
@@ -3868,19 +3868,19 @@
       <c r="D56" s="1"/>
       <c r="K56" s="54">
         <f>IFERROR(K55/$D$55, 0)</f>
-        <v>0.28146733288804565</v>
+        <v>0.27602901579233796</v>
       </c>
       <c r="L56" s="54">
         <f>IFERROR(L55/$D$55, 0)</f>
-        <v>0.67654973049932998</v>
+        <v>0.68479060064071307</v>
       </c>
       <c r="M56" s="54">
         <f>IFERROR(M55/$D$55, 0)</f>
-        <v>3.7744151730957215E-2</v>
+        <v>3.5224556964015122E-2</v>
       </c>
       <c r="N56" s="54">
         <f>IFERROR(N55/$D$55, 0)</f>
-        <v>3.1453459775797679E-3</v>
+        <v>2.93537974700126E-3</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
@@ -4094,7 +4094,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P9" sqref="P9:P44"/>
+      <selection pane="bottomRight" activeCell="O9" sqref="O9:O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4644,15 +4644,15 @@
       </c>
       <c r="M9" s="65">
         <f>$F9*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N9" s="65">
         <f>$F9*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O9" s="65">
         <f>$F9*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P9" s="65">
         <f>$F9*Outputs_Internal!M$52/12</f>
@@ -4718,15 +4718,15 @@
       </c>
       <c r="M10" s="65">
         <f>$F10*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N10" s="65">
         <f>$F10*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O10" s="65">
         <f>$F10*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P10" s="65">
         <f>$F10*Outputs_Internal!M$52/12</f>
@@ -4792,15 +4792,15 @@
       </c>
       <c r="M11" s="65">
         <f>$F11*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N11" s="65">
         <f>$F11*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O11" s="65">
         <f>$F11*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P11" s="65">
         <f>$F11*Outputs_Internal!M$52/12</f>
@@ -4812,15 +4812,15 @@
       </c>
       <c r="S11" s="65">
         <f t="shared" si="2"/>
-        <v>28175</v>
+        <v>29862.5</v>
       </c>
       <c r="T11" s="65">
         <f t="shared" si="3"/>
-        <v>8931.9501617171445</v>
+        <v>9269.4501617171445</v>
       </c>
       <c r="U11" s="65">
         <f>IF(MOD(MONTH($B11),3)=0,SUM(J9:J11,O9:O11),0)</f>
-        <v>18252.602392030025</v>
+        <v>19602.602392030021</v>
       </c>
       <c r="V11" s="65">
         <f t="shared" si="4"/>
@@ -4866,15 +4866,15 @@
       </c>
       <c r="M12" s="65">
         <f>$F12*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N12" s="65">
         <f>$F12*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O12" s="65">
         <f>$F12*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P12" s="65">
         <f>$F12*Outputs_Internal!M$52/12</f>
@@ -4940,15 +4940,15 @@
       </c>
       <c r="M13" s="65">
         <f>$F13*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N13" s="65">
         <f>$F13*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O13" s="65">
         <f>$F13*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P13" s="65">
         <f>$F13*Outputs_Internal!M$52/12</f>
@@ -5014,15 +5014,15 @@
       </c>
       <c r="M14" s="65">
         <f>$F14*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N14" s="65">
         <f>$F14*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O14" s="65">
         <f>$F14*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P14" s="65">
         <f>$F14*Outputs_Internal!M$52/12</f>
@@ -5034,15 +5034,15 @@
       </c>
       <c r="S14" s="65">
         <f t="shared" si="2"/>
-        <v>23175</v>
+        <v>24862.5</v>
       </c>
       <c r="T14" s="65">
         <f t="shared" si="3"/>
-        <v>6431.9501617171427</v>
+        <v>6769.4501617171427</v>
       </c>
       <c r="U14" s="65">
         <f t="shared" si="4"/>
-        <v>15752.602392030025</v>
+        <v>17102.602392030025</v>
       </c>
       <c r="V14" s="65">
         <f t="shared" si="4"/>
@@ -5088,15 +5088,15 @@
       </c>
       <c r="M15" s="65">
         <f>$F15*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N15" s="65">
         <f>$F15*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O15" s="65">
         <f>$F15*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P15" s="65">
         <f>$F15*Outputs_Internal!M$52/12</f>
@@ -5162,15 +5162,15 @@
       </c>
       <c r="M16" s="65">
         <f>$F16*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N16" s="65">
         <f>$F16*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O16" s="65">
         <f>$F16*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P16" s="65">
         <f>$F16*Outputs_Internal!M$52/12</f>
@@ -5236,15 +5236,15 @@
       </c>
       <c r="M17" s="65">
         <f>$F17*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N17" s="65">
         <f>$F17*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O17" s="65">
         <f>$F17*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P17" s="65">
         <f>$F17*Outputs_Internal!M$52/12</f>
@@ -5256,15 +5256,15 @@
       </c>
       <c r="S17" s="65">
         <f t="shared" si="2"/>
-        <v>23175</v>
+        <v>24862.5</v>
       </c>
       <c r="T17" s="65">
         <f t="shared" si="3"/>
-        <v>6431.9501617171427</v>
+        <v>6769.4501617171427</v>
       </c>
       <c r="U17" s="65">
         <f t="shared" si="4"/>
-        <v>15752.602392030025</v>
+        <v>17102.602392030025</v>
       </c>
       <c r="V17" s="65">
         <f t="shared" si="4"/>
@@ -5310,15 +5310,15 @@
       </c>
       <c r="M18" s="65">
         <f>$F18*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N18" s="65">
         <f>$F18*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O18" s="65">
         <f>$F18*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P18" s="65">
         <f>$F18*Outputs_Internal!M$52/12</f>
@@ -5384,15 +5384,15 @@
       </c>
       <c r="M19" s="65">
         <f>$F19*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N19" s="65">
         <f>$F19*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O19" s="65">
         <f>$F19*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P19" s="65">
         <f>$F19*Outputs_Internal!M$52/12</f>
@@ -5458,15 +5458,15 @@
       </c>
       <c r="M20" s="65">
         <f>$F20*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N20" s="65">
         <f>$F20*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O20" s="65">
         <f>$F20*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P20" s="65">
         <f>$F20*Outputs_Internal!M$52/12</f>
@@ -5478,15 +5478,15 @@
       </c>
       <c r="S20" s="65">
         <f t="shared" si="2"/>
-        <v>23175</v>
+        <v>24862.5</v>
       </c>
       <c r="T20" s="65">
         <f t="shared" si="3"/>
-        <v>6431.9501617171427</v>
+        <v>6769.4501617171427</v>
       </c>
       <c r="U20" s="65">
         <f t="shared" si="4"/>
-        <v>15752.602392030025</v>
+        <v>17102.602392030025</v>
       </c>
       <c r="V20" s="65">
         <f t="shared" si="4"/>
@@ -5532,15 +5532,15 @@
       </c>
       <c r="M21" s="65">
         <f>$F21*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N21" s="65">
         <f>$F21*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O21" s="65">
         <f>$F21*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P21" s="65">
         <f>$F21*Outputs_Internal!M$52/12</f>
@@ -5606,15 +5606,15 @@
       </c>
       <c r="M22" s="65">
         <f>$F22*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N22" s="65">
         <f>$F22*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O22" s="65">
         <f>$F22*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P22" s="65">
         <f>$F22*Outputs_Internal!M$52/12</f>
@@ -5680,15 +5680,15 @@
       </c>
       <c r="M23" s="65">
         <f>$F23*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N23" s="65">
         <f>$F23*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O23" s="65">
         <f>$F23*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P23" s="65">
         <f>$F23*Outputs_Internal!M$52/12</f>
@@ -5700,15 +5700,15 @@
       </c>
       <c r="S23" s="65">
         <f t="shared" si="2"/>
-        <v>23175</v>
+        <v>24862.5</v>
       </c>
       <c r="T23" s="65">
         <f t="shared" si="3"/>
-        <v>6431.9501617171427</v>
+        <v>6769.4501617171427</v>
       </c>
       <c r="U23" s="65">
         <f t="shared" si="4"/>
-        <v>15752.602392030025</v>
+        <v>17102.602392030025</v>
       </c>
       <c r="V23" s="65">
         <f t="shared" si="4"/>
@@ -5754,15 +5754,15 @@
       </c>
       <c r="M24" s="65">
         <f>$F24*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N24" s="65">
         <f>$F24*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O24" s="65">
         <f>$F24*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P24" s="65">
         <f>$F24*Outputs_Internal!M$52/12</f>
@@ -5828,15 +5828,15 @@
       </c>
       <c r="M25" s="65">
         <f>$F25*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N25" s="65">
         <f>$F25*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O25" s="65">
         <f>$F25*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P25" s="65">
         <f>$F25*Outputs_Internal!M$52/12</f>
@@ -5902,15 +5902,15 @@
       </c>
       <c r="M26" s="65">
         <f>$F26*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N26" s="65">
         <f>$F26*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O26" s="65">
         <f>$F26*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P26" s="65">
         <f>$F26*Outputs_Internal!M$52/12</f>
@@ -5922,15 +5922,15 @@
       </c>
       <c r="S26" s="65">
         <f t="shared" si="2"/>
-        <v>23175</v>
+        <v>24862.5</v>
       </c>
       <c r="T26" s="65">
         <f t="shared" si="3"/>
-        <v>6431.9501617171427</v>
+        <v>6769.4501617171427</v>
       </c>
       <c r="U26" s="65">
         <f t="shared" si="4"/>
-        <v>15752.602392030025</v>
+        <v>17102.602392030025</v>
       </c>
       <c r="V26" s="65">
         <f t="shared" si="4"/>
@@ -5976,15 +5976,15 @@
       </c>
       <c r="M27" s="65">
         <f>$F27*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N27" s="65">
         <f>$F27*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O27" s="65">
         <f>$F27*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P27" s="65">
         <f>$F27*Outputs_Internal!M$52/12</f>
@@ -6050,15 +6050,15 @@
       </c>
       <c r="M28" s="65">
         <f>$F28*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N28" s="65">
         <f>$F28*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O28" s="65">
         <f>$F28*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P28" s="65">
         <f>$F28*Outputs_Internal!M$52/12</f>
@@ -6124,15 +6124,15 @@
       </c>
       <c r="M29" s="65">
         <f>$F29*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N29" s="65">
         <f>$F29*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O29" s="65">
         <f>$F29*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P29" s="65">
         <f>$F29*Outputs_Internal!M$52/12</f>
@@ -6144,15 +6144,15 @@
       </c>
       <c r="S29" s="65">
         <f t="shared" si="2"/>
-        <v>23175</v>
+        <v>24862.5</v>
       </c>
       <c r="T29" s="65">
         <f t="shared" si="3"/>
-        <v>6431.9501617171427</v>
+        <v>6769.4501617171427</v>
       </c>
       <c r="U29" s="65">
         <f t="shared" si="4"/>
-        <v>15752.602392030025</v>
+        <v>17102.602392030025</v>
       </c>
       <c r="V29" s="65">
         <f t="shared" si="4"/>
@@ -6198,15 +6198,15 @@
       </c>
       <c r="M30" s="65">
         <f>$F30*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N30" s="65">
         <f>$F30*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O30" s="65">
         <f>$F30*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P30" s="65">
         <f>$F30*Outputs_Internal!M$52/12</f>
@@ -6272,15 +6272,15 @@
       </c>
       <c r="M31" s="65">
         <f>$F31*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N31" s="65">
         <f>$F31*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O31" s="65">
         <f>$F31*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P31" s="65">
         <f>$F31*Outputs_Internal!M$52/12</f>
@@ -6346,15 +6346,15 @@
       </c>
       <c r="M32" s="65">
         <f>$F32*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N32" s="65">
         <f>$F32*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O32" s="65">
         <f>$F32*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P32" s="65">
         <f>$F32*Outputs_Internal!M$52/12</f>
@@ -6366,15 +6366,15 @@
       </c>
       <c r="S32" s="65">
         <f t="shared" si="2"/>
-        <v>23175</v>
+        <v>24862.5</v>
       </c>
       <c r="T32" s="65">
         <f t="shared" si="3"/>
-        <v>6431.9501617171427</v>
+        <v>6769.4501617171427</v>
       </c>
       <c r="U32" s="65">
         <f t="shared" si="4"/>
-        <v>15752.602392030025</v>
+        <v>17102.602392030025</v>
       </c>
       <c r="V32" s="65">
         <f t="shared" si="4"/>
@@ -6420,15 +6420,15 @@
       </c>
       <c r="M33" s="65">
         <f>$F33*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N33" s="65">
         <f>$F33*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O33" s="65">
         <f>$F33*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P33" s="65">
         <f>$F33*Outputs_Internal!M$52/12</f>
@@ -6494,15 +6494,15 @@
       </c>
       <c r="M34" s="65">
         <f>$F34*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N34" s="65">
         <f>$F34*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O34" s="65">
         <f>$F34*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P34" s="65">
         <f>$F34*Outputs_Internal!M$52/12</f>
@@ -6568,15 +6568,15 @@
       </c>
       <c r="M35" s="65">
         <f>$F35*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N35" s="65">
         <f>$F35*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O35" s="65">
         <f>$F35*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P35" s="65">
         <f>$F35*Outputs_Internal!M$52/12</f>
@@ -6588,15 +6588,15 @@
       </c>
       <c r="S35" s="65">
         <f t="shared" si="2"/>
-        <v>23175</v>
+        <v>24862.5</v>
       </c>
       <c r="T35" s="65">
         <f t="shared" si="3"/>
-        <v>6431.9501617171427</v>
+        <v>6769.4501617171427</v>
       </c>
       <c r="U35" s="65">
         <f t="shared" si="4"/>
-        <v>15752.602392030025</v>
+        <v>17102.602392030025</v>
       </c>
       <c r="V35" s="65">
         <f t="shared" si="4"/>
@@ -6642,15 +6642,15 @@
       </c>
       <c r="M36" s="65">
         <f>$F36*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N36" s="65">
         <f>$F36*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O36" s="65">
         <f>$F36*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P36" s="65">
         <f>$F36*Outputs_Internal!M$52/12</f>
@@ -6716,15 +6716,15 @@
       </c>
       <c r="M37" s="65">
         <f>$F37*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N37" s="65">
         <f>$F37*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O37" s="65">
         <f>$F37*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P37" s="65">
         <f>$F37*Outputs_Internal!M$52/12</f>
@@ -6790,15 +6790,15 @@
       </c>
       <c r="M38" s="65">
         <f>$F38*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N38" s="65">
         <f>$F38*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O38" s="65">
         <f>$F38*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P38" s="65">
         <f>$F38*Outputs_Internal!M$52/12</f>
@@ -6810,15 +6810,15 @@
       </c>
       <c r="S38" s="65">
         <f t="shared" si="2"/>
-        <v>23175</v>
+        <v>24862.5</v>
       </c>
       <c r="T38" s="65">
         <f t="shared" si="3"/>
-        <v>6431.9501617171427</v>
+        <v>6769.4501617171427</v>
       </c>
       <c r="U38" s="65">
         <f t="shared" si="4"/>
-        <v>15752.602392030025</v>
+        <v>17102.602392030025</v>
       </c>
       <c r="V38" s="65">
         <f t="shared" si="4"/>
@@ -6864,15 +6864,15 @@
       </c>
       <c r="M39" s="65">
         <f>$F39*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N39" s="65">
         <f>$F39*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O39" s="65">
         <f>$F39*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P39" s="65">
         <f>$F39*Outputs_Internal!M$52/12</f>
@@ -6938,15 +6938,15 @@
       </c>
       <c r="M40" s="65">
         <f>$F40*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N40" s="65">
         <f>$F40*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O40" s="65">
         <f>$F40*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P40" s="65">
         <f>$F40*Outputs_Internal!M$52/12</f>
@@ -7012,15 +7012,15 @@
       </c>
       <c r="M41" s="65">
         <f>$F41*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N41" s="65">
         <f>$F41*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O41" s="65">
         <f>$F41*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P41" s="65">
         <f>$F41*Outputs_Internal!M$52/12</f>
@@ -7032,15 +7032,15 @@
       </c>
       <c r="S41" s="65">
         <f t="shared" si="2"/>
-        <v>23175</v>
+        <v>24862.5</v>
       </c>
       <c r="T41" s="65">
         <f t="shared" si="3"/>
-        <v>6431.9501617171427</v>
+        <v>6769.4501617171427</v>
       </c>
       <c r="U41" s="65">
         <f t="shared" si="4"/>
-        <v>15752.602392030025</v>
+        <v>17102.602392030025</v>
       </c>
       <c r="V41" s="65">
         <f t="shared" si="4"/>
@@ -7086,15 +7086,15 @@
       </c>
       <c r="M42" s="65">
         <f>$F42*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N42" s="65">
         <f>$F42*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O42" s="65">
         <f>$F42*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P42" s="65">
         <f>$F42*Outputs_Internal!M$52/12</f>
@@ -7160,15 +7160,15 @@
       </c>
       <c r="M43" s="65">
         <f>$F43*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N43" s="65">
         <f>$F43*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O43" s="65">
         <f>$F43*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P43" s="65">
         <f>$F43*Outputs_Internal!M$52/12</f>
@@ -7234,15 +7234,15 @@
       </c>
       <c r="M44" s="65">
         <f>$F44*Outputs_Internal!$D$52/12</f>
-        <v>7725</v>
+        <v>8287.5</v>
       </c>
       <c r="N44" s="65">
         <f>$F44*Outputs_Internal!K$52/12</f>
-        <v>2143.9833872390477</v>
+        <v>2256.4833872390477</v>
       </c>
       <c r="O44" s="65">
         <f>$F44*Outputs_Internal!L$52/12</f>
-        <v>5250.867464010008</v>
+        <v>5700.867464010008</v>
       </c>
       <c r="P44" s="65">
         <f>$F44*Outputs_Internal!M$52/12</f>
@@ -7254,15 +7254,15 @@
       </c>
       <c r="S44" s="65">
         <f>IF(MOD(MONTH($B44),3)=0,SUM(H42:H44,M42:M44),0)</f>
-        <v>23175</v>
+        <v>24862.5</v>
       </c>
       <c r="T44" s="65">
         <f t="shared" si="3"/>
-        <v>6431.9501617171427</v>
+        <v>6769.4501617171427</v>
       </c>
       <c r="U44" s="65">
         <f t="shared" si="4"/>
-        <v>15752.602392030025</v>
+        <v>17102.602392030025</v>
       </c>
       <c r="V44" s="65">
         <f t="shared" si="4"/>
@@ -11155,7 +11155,7 @@
       </c>
       <c r="D10" s="16">
         <f>IF(Inputs!D8="Y", Prices!$C$7, 0)</f>
-        <v>0</v>
+        <v>6750</v>
       </c>
       <c r="E10" s="16">
         <f>IF(Inputs!E8="Y", Prices!$C$7, 0)</f>
@@ -11712,7 +11712,7 @@
       </c>
       <c r="D36" s="16">
         <f>IF(Inputs!D8="Y", Prices!$C$7, 0)</f>
-        <v>0</v>
+        <v>6750</v>
       </c>
       <c r="E36" s="16">
         <f>IF(Inputs!E8="Y", Prices!$C$7, 0)</f>
@@ -12824,7 +12824,7 @@
       </c>
       <c r="D88" s="7">
         <f>SUM(D35:D45, D48:D58, D61:D64, D67:D70, D85:D86)</f>
-        <v>92700</v>
+        <v>99450</v>
       </c>
       <c r="E88" s="7">
         <f t="shared" ref="E88:H88" si="20">SUM(E35:E45, E48:E58, E61:E64, E67:E70, E85:E86)</f>
@@ -12909,7 +12909,7 @@
       </c>
       <c r="D94" s="7">
         <f>SUM(D88, D90)</f>
-        <v>92700</v>
+        <v>99450</v>
       </c>
       <c r="E94" s="7">
         <f>SUM(E88, E90)</f>

</xml_diff>